<commit_message>
Added column + binary search tests
Signed-off-by: JaDogg <JaDogg@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\java-perf-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6237CF-FC25-46A0-810E-C536413D0ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA780BF2-834C-4728-BE82-F3BFFB0E9176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{01CF522D-6A49-4C1C-95FD-0E9005DE6AAD}"/>
   </bookViews>
@@ -35,15 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Count</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
-    <t>Map</t>
   </si>
   <si>
     <t>Object lookup from ID</t>
@@ -52,19 +46,49 @@
     <t>Object lookup from name</t>
   </si>
   <si>
-    <t>Array Sorted</t>
-  </si>
-  <si>
     <t>Contains Integer</t>
   </si>
   <si>
-    <t>Map ContainsKey</t>
+    <t>searchArray</t>
   </si>
   <si>
-    <t>Map GetOrDefault</t>
+    <t>searchWithHash</t>
   </si>
   <si>
-    <t>Set Contains</t>
+    <t>fromMap</t>
+  </si>
+  <si>
+    <t>searchArrayNaiveSorted</t>
+  </si>
+  <si>
+    <t>searchArrayNaiveUnsorted</t>
+  </si>
+  <si>
+    <t>searchBinarySearch</t>
+  </si>
+  <si>
+    <t>searchWithHashPersonColumns</t>
+  </si>
+  <si>
+    <t>searchColumnNaiveSearch</t>
+  </si>
+  <si>
+    <t>searchColumnsBinarySearch</t>
+  </si>
+  <si>
+    <t>fromSet</t>
+  </si>
+  <si>
+    <t>searchArraySorted</t>
+  </si>
+  <si>
+    <t>searchArrayUnsorted</t>
+  </si>
+  <si>
+    <t>fromMapGet</t>
+  </si>
+  <si>
+    <t>fromMapContainsKey</t>
   </si>
 </sst>
 </file>
@@ -106,11 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,16 +178,45 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Array</c:v>
+            <c:v>searchArray</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -190,13 +244,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4544518.5279999999</c:v>
+                  <c:v>5066162.8789999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2399776.0860000001</c:v>
+                  <c:v>2298710.2510000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1626677.0689999999</c:v>
+                  <c:v>1678781.9069999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -208,19 +262,189 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Map</c:v>
+            <c:v>searchWithHash</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>ObjectFromName!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8266041.3569999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4721242.1629999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3493189.341</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC12-4736-BAB9-E46DE5D265AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>searchWithHashPersonColumns</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>ObjectFromName!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7823327.0180000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5094816.3729999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3279703.7910000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EC12-4736-BAB9-E46DE5D265AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>fromMap</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -248,13 +472,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15819679.961999999</c:v>
+                  <c:v>16107658.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15568455.35</c:v>
+                  <c:v>15498049.169</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16284080.539000001</c:v>
+                  <c:v>15959047.493000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -273,7 +497,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="711960303"/>
         <c:axId val="703459583"/>
       </c:barChart>
@@ -291,11 +516,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -323,11 +547,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -345,11 +568,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -363,9 +586,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -394,9 +616,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -411,11 +633,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -443,11 +664,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -477,9 +697,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -519,9 +738,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -545,17 +763,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -602,16 +831,45 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Array</c:v>
+            <c:v>searchArrayNaiveUnsorted</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -639,13 +897,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>17729478.116</c:v>
+                  <c:v>18803849.857000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12171721.524</c:v>
+                  <c:v>12017715.333000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8767859.2090000007</c:v>
+                  <c:v>9552699.8760000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,16 +918,45 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Map</c:v>
+            <c:v>searchArrayNaiveSorted</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -697,13 +984,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14409324.452</c:v>
+                  <c:v>17184658.219999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14093965.617000001</c:v>
+                  <c:v>12110462.143999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14555449.124</c:v>
+                  <c:v>8881557.2080000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -718,16 +1005,45 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Array Sorted</c:v>
+            <c:v>searchBinarySearch</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -737,13 +1053,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19073751.006000001</c:v>
+                  <c:v>11897310.188999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12204679.927999999</c:v>
+                  <c:v>11133821.339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9249547.8300000001</c:v>
+                  <c:v>9601265.8269999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -751,6 +1067,222 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9FEC-4C52-AFC0-A8A18FB65D7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>fromMap</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>ObjectFromID!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>14866381.397</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13369362.194</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14985075.044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F36B-475E-B0A9-298A12EEF6FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>searchColumnNaiveSearch</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>ObjectFromID!$F$3:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20315752.302000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14687363.204</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11076919.111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F36B-475E-B0A9-298A12EEF6FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>searchColumnBinarySearch</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>ObjectFromID!$G$3:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16337186.915999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13384558.130000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13263050.884</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F36B-475E-B0A9-298A12EEF6FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -762,7 +1294,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="711960303"/>
         <c:axId val="703459583"/>
       </c:barChart>
@@ -780,11 +1313,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -812,11 +1344,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -834,11 +1365,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -852,9 +1383,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -883,9 +1413,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -900,11 +1430,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -932,11 +1461,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -966,9 +1494,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1008,9 +1535,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1034,17 +1560,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1091,24 +1628,53 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Array</c:v>
+            <c:v>searchArrayUnsorted</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>ContainsInteger!$A$3:$A$5</c:f>
+              <c:f>ContainsInteger!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1117,24 +1683,30 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ContainsInteger!$B$3:$B$5</c:f>
+              <c:f>ContainsInteger!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20410552.877</c:v>
+                  <c:v>20122808.188999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15033859.645</c:v>
+                  <c:v>14541830.884</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11549358.780999999</c:v>
+                  <c:v>11438309.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10097456.539999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1149,32 +1721,85 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>ArraySorted</c:v>
+            <c:v>searchArraySorted</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ContainsInteger!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ContainsInteger!$D$3:$D$5</c:f>
+              <c:f>ContainsInteger!$D$3:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>19933675.184</c:v>
+                  <c:v>19239907.842</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14087577.666999999</c:v>
+                  <c:v>15041980.968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11307742</c:v>
+                  <c:v>11493418.448999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9391938.9370000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1189,24 +1814,53 @@
           <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>MapContainsK</c:v>
+            <c:v>fromMapContainsKey</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>ContainsInteger!$A$3:$A$5</c:f>
+              <c:f>ContainsInteger!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1215,24 +1869,30 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ContainsInteger!$C$3:$C$5</c:f>
+              <c:f>ContainsInteger!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14375144.806</c:v>
+                  <c:v>15251857.493000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15258375.335000001</c:v>
+                  <c:v>14522563.115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15524192.397</c:v>
+                  <c:v>15428368.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15547405.876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1247,32 +1907,88 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>MapGet</c:v>
+            <c:v>fromMapGet</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ContainsInteger!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ContainsInteger!$E$3:$E$5</c:f>
+              <c:f>ContainsInteger!$E$3:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13522687.822000001</c:v>
+                  <c:v>13716313.130999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13680914.325999999</c:v>
+                  <c:v>13978913.697000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14042773.282</c:v>
+                  <c:v>14081918.014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13789620.162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,32 +2003,88 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>SetContains</c:v>
+            <c:v>fromSet</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ContainsInteger!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ContainsInteger!$F$3:$F$5</c:f>
+              <c:f>ContainsInteger!$F$3:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14464775.118000001</c:v>
+                  <c:v>14608768.215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14509041.697000001</c:v>
+                  <c:v>14613174.528999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14688918.193</c:v>
+                  <c:v>14534259.816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14830772.289000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,6 +2092,102 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3466-4469-97B7-616267FAF25F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>searchBinarySearch</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ContainsInteger!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ContainsInteger!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15735621.665999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15743363.713</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14669313.561000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13523277.487</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A964-42E3-B69A-8E94E005605B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1331,7 +2199,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="711960303"/>
         <c:axId val="703459583"/>
       </c:barChart>
@@ -1349,11 +2218,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1381,11 +2249,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1403,11 +2270,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1421,9 +2288,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1452,9 +2318,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1469,11 +2335,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1501,11 +2366,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1535,9 +2399,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1577,9 +2440,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1603,17 +2465,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1636,13 +2509,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1676,13 +2546,10 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1716,13 +2583,10 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1756,35 +2620,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1792,26 +2654,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1820,9 +2690,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1841,14 +2710,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1857,45 +2718,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1907,33 +2758,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1949,21 +2798,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1973,20 +2819,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1997,167 +2843,167 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2165,14 +3011,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2184,12 +3030,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2198,14 +3051,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2214,9 +3066,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2226,7 +3077,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2234,9 +3085,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2247,9 +3098,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2259,48 +3109,40 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2308,26 +3150,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -2336,9 +3186,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2357,14 +3206,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2373,45 +3214,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2423,33 +3254,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2465,21 +3294,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2489,20 +3315,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2513,167 +3339,167 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2681,14 +3507,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2700,12 +3526,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2714,14 +3547,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2730,9 +3562,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2742,7 +3573,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2750,9 +3581,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2763,9 +3594,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2775,48 +3605,40 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2824,26 +3646,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -2852,9 +3682,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2873,14 +3702,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2889,45 +3710,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2939,33 +3750,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2981,21 +3790,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3005,20 +3811,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3029,167 +3835,167 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3197,14 +4003,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3216,12 +4022,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3230,14 +4043,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3246,9 +4058,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3258,7 +4069,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3266,9 +4077,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3279,9 +4090,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3291,14 +4101,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3308,15 +4112,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>111673</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>6569</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>81784</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>82769</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3349,15 +4153,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>210207</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19707</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>791232</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>95907</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3392,15 +4196,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>164224</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>124810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>745249</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>10510</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3730,7 +4534,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3738,11 +4542,13 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3755,10 +4561,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3766,10 +4578,16 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>4544518.5279999999</v>
+        <v>5066162.8789999997</v>
       </c>
       <c r="C3">
-        <v>15819679.961999999</v>
+        <v>16107658.4</v>
+      </c>
+      <c r="D3">
+        <v>8266041.3569999998</v>
+      </c>
+      <c r="E3">
+        <v>7823327.0180000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3777,10 +4595,16 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>2399776.0860000001</v>
+        <v>2298710.2510000002</v>
       </c>
       <c r="C4">
-        <v>15568455.35</v>
+        <v>15498049.169</v>
+      </c>
+      <c r="D4">
+        <v>4721242.1629999997</v>
+      </c>
+      <c r="E4">
+        <v>5094816.3729999997</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3788,10 +4612,16 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>1626677.0689999999</v>
+        <v>1678781.9069999999</v>
       </c>
       <c r="C5">
-        <v>16284080.539000001</v>
+        <v>15959047.493000001</v>
+      </c>
+      <c r="D5">
+        <v>3493189.341</v>
+      </c>
+      <c r="E5">
+        <v>3279703.7910000002</v>
       </c>
     </row>
   </sheetData>
@@ -3805,206 +4635,284 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B943DCBB-F5D0-42FE-BB01-1BF06733AE66}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>17729478.116</v>
+        <v>18803849.857000001</v>
       </c>
       <c r="C3">
-        <v>14409324.452</v>
+        <v>17184658.219999999</v>
       </c>
       <c r="D3">
-        <v>19073751.006000001</v>
+        <v>11897310.188999999</v>
+      </c>
+      <c r="E3">
+        <v>14866381.397</v>
+      </c>
+      <c r="F3">
+        <v>20315752.302000001</v>
+      </c>
+      <c r="G3">
+        <v>16337186.915999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
       <c r="B4">
-        <v>12171721.524</v>
+        <v>12017715.333000001</v>
       </c>
       <c r="C4">
-        <v>14093965.617000001</v>
+        <v>12110462.143999999</v>
       </c>
       <c r="D4">
-        <v>12204679.927999999</v>
+        <v>11133821.339</v>
+      </c>
+      <c r="E4">
+        <v>13369362.194</v>
+      </c>
+      <c r="F4">
+        <v>14687363.204</v>
+      </c>
+      <c r="G4">
+        <v>13384558.130000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
       <c r="B5">
-        <v>8767859.2090000007</v>
+        <v>9552699.8760000002</v>
       </c>
       <c r="C5">
-        <v>14555449.124</v>
+        <v>8881557.2080000006</v>
       </c>
       <c r="D5">
-        <v>9249547.8300000001</v>
+        <v>9601265.8269999996</v>
+      </c>
+      <c r="E5">
+        <v>14985075.044</v>
+      </c>
+      <c r="F5">
+        <v>11076919.111</v>
+      </c>
+      <c r="G5">
+        <v>13263050.884</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25B610C-994E-4C7B-A018-A057F1FE4C82}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>20410552.877</v>
-      </c>
-      <c r="C3">
-        <v>14375144.806</v>
+        <v>20122808.188999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15251857.493000001</v>
       </c>
       <c r="D3">
-        <v>19933675.184</v>
+        <v>19239907.842</v>
       </c>
       <c r="E3">
-        <v>13522687.822000001</v>
+        <v>13716313.130999999</v>
       </c>
       <c r="F3">
-        <v>14464775.118000001</v>
+        <v>14608768.215</v>
+      </c>
+      <c r="G3">
+        <v>15735621.665999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
       <c r="B4">
-        <v>15033859.645</v>
+        <v>14541830.884</v>
       </c>
       <c r="C4">
-        <v>15258375.335000001</v>
+        <v>14522563.115</v>
       </c>
       <c r="D4">
-        <v>14087577.666999999</v>
+        <v>15041980.968</v>
       </c>
       <c r="E4">
-        <v>13680914.325999999</v>
+        <v>13978913.697000001</v>
       </c>
       <c r="F4">
-        <v>14509041.697000001</v>
+        <v>14613174.528999999</v>
+      </c>
+      <c r="G4">
+        <v>15743363.713</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
       <c r="B5">
-        <v>11549358.780999999</v>
+        <v>11438309.92</v>
       </c>
       <c r="C5">
-        <v>15524192.397</v>
+        <v>15428368.82</v>
       </c>
       <c r="D5">
-        <v>11307742</v>
+        <v>11493418.448999999</v>
       </c>
       <c r="E5">
-        <v>14042773.282</v>
+        <v>14081918.014</v>
       </c>
       <c r="F5">
-        <v>14688918.193</v>
+        <v>14534259.816</v>
+      </c>
+      <c r="G5">
+        <v>14669313.561000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>10097456.539999999</v>
+      </c>
+      <c r="C6">
+        <v>15547405.876</v>
+      </c>
+      <c r="D6">
+        <v>9391938.9370000008</v>
+      </c>
+      <c r="E6">
+        <v>13789620.162</v>
+      </c>
+      <c r="F6">
+        <v>14830772.289000001</v>
+      </c>
+      <c r="G6">
+        <v>13523277.487</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>